<commit_message>
fix: creating a specific excel file to prediction with prod_E and prod_L
</commit_message>
<xml_diff>
--- a/results/input_data/prediction_data_original.xlsx
+++ b/results/input_data/prediction_data_original.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">potencia boosting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prod_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prod_l</t>
   </si>
 </sst>
 </file>
@@ -181,8 +175,8 @@
   </sheetPr>
   <dimension ref="A1:R367"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1:I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -215,12 +209,8 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -244,12 +234,6 @@
       <c r="G2" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -274,12 +258,6 @@
       <c r="G3" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,12 +282,6 @@
       <c r="G4" s="3" t="n">
         <v>1.3</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,12 +306,6 @@
       <c r="G5" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,12 +330,6 @@
       <c r="G6" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,12 +354,6 @@
       <c r="G7" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,12 +378,6 @@
       <c r="G8" s="3" t="n">
         <v>1.4</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,12 +402,6 @@
       <c r="G9" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,12 +426,6 @@
       <c r="G10" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,12 +450,6 @@
       <c r="G11" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,12 +474,6 @@
       <c r="G12" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,12 +498,6 @@
       <c r="G13" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,12 +522,6 @@
       <c r="G14" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -634,12 +546,6 @@
       <c r="G15" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,12 +570,6 @@
       <c r="G16" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,12 +594,6 @@
       <c r="G17" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -724,12 +618,6 @@
       <c r="G18" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,12 +642,6 @@
       <c r="G19" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="H19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -784,12 +666,6 @@
       <c r="G20" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,12 +690,6 @@
       <c r="G21" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,12 +714,6 @@
       <c r="G22" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,12 +738,6 @@
       <c r="G23" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -904,12 +762,6 @@
       <c r="G24" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,12 +786,6 @@
       <c r="G25" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,12 +810,6 @@
       <c r="G26" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,12 +834,6 @@
       <c r="G27" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1024,12 +858,6 @@
       <c r="G28" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,12 +882,6 @@
       <c r="G29" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1084,12 +906,6 @@
       <c r="G30" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,12 +930,6 @@
       <c r="G31" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,12 +954,6 @@
       <c r="G32" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,12 +978,6 @@
       <c r="G33" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,12 +1002,6 @@
       <c r="G34" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H34" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,12 +1026,6 @@
       <c r="G35" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H35" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,12 +1050,6 @@
       <c r="G36" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,12 +1074,6 @@
       <c r="G37" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,12 +1098,6 @@
       <c r="G38" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H38" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,12 +1122,6 @@
       <c r="G39" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H39" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,12 +1146,6 @@
       <c r="G40" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I40" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1414,12 +1170,6 @@
       <c r="G41" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,12 +1194,6 @@
       <c r="G42" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,12 +1218,6 @@
       <c r="G43" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1504,12 +1242,6 @@
       <c r="G44" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,12 +1266,6 @@
       <c r="G45" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,12 +1290,6 @@
       <c r="G46" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,12 +1314,6 @@
       <c r="G47" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,12 +1338,6 @@
       <c r="G48" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I48" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,12 +1362,6 @@
       <c r="G49" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H49" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I49" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,12 +1386,6 @@
       <c r="G50" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H50" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I50" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,12 +1410,6 @@
       <c r="G51" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H51" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I51" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,12 +1434,6 @@
       <c r="G52" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H52" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,12 +1458,6 @@
       <c r="G53" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H53" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I53" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,12 +1482,6 @@
       <c r="G54" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,12 +1506,6 @@
       <c r="G55" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H55" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,12 +1530,6 @@
       <c r="G56" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H56" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,12 +1554,6 @@
       <c r="G57" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I57" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,12 +1578,6 @@
       <c r="G58" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I58" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,12 +1602,6 @@
       <c r="G59" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I59" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,12 +1626,6 @@
       <c r="G60" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I60" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,12 +1650,6 @@
       <c r="G61" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I61" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2044,12 +1674,6 @@
       <c r="G62" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H62" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I62" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2074,12 +1698,6 @@
       <c r="G63" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H63" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I63" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,12 +1722,6 @@
       <c r="G64" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H64" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I64" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2134,12 +1746,6 @@
       <c r="G65" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H65" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I65" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,12 +1770,6 @@
       <c r="G66" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H66" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,12 +1794,6 @@
       <c r="G67" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H67" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I67" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,12 +1818,6 @@
       <c r="G68" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H68" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I68" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,12 +1842,6 @@
       <c r="G69" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H69" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I69" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,12 +1866,6 @@
       <c r="G70" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H70" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I70" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,12 +1890,6 @@
       <c r="G71" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H71" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I71" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,12 +1914,6 @@
       <c r="G72" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H72" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I72" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2374,12 +1938,6 @@
       <c r="G73" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I73" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,12 +1962,6 @@
       <c r="G74" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I74" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,12 +1986,6 @@
       <c r="G75" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2464,12 +2010,6 @@
       <c r="G76" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I76" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2494,12 +2034,6 @@
       <c r="G77" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H77" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I77" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,12 +2058,6 @@
       <c r="G78" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H78" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I78" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,12 +2082,6 @@
       <c r="G79" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H79" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I79" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2584,12 +2106,6 @@
       <c r="G80" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I80" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2614,12 +2130,6 @@
       <c r="G81" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H81" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I81" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,12 +2154,6 @@
       <c r="G82" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H82" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I82" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,12 +2178,6 @@
       <c r="G83" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H83" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I83" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,12 +2202,6 @@
       <c r="G84" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H84" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I84" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,12 +2226,6 @@
       <c r="G85" s="3" t="n">
         <v>1.8</v>
       </c>
-      <c r="H85" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I85" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2764,12 +2250,6 @@
       <c r="G86" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H86" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,12 +2274,6 @@
       <c r="G87" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H87" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I87" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2824,12 +2298,6 @@
       <c r="G88" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H88" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I88" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,12 +2322,6 @@
       <c r="G89" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H89" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I89" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="R89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,12 +2346,6 @@
       <c r="G90" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H90" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I90" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,12 +2370,6 @@
       <c r="G91" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="H91" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I91" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="R91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,12 +2393,6 @@
       </c>
       <c r="G92" s="3" t="n">
         <v>3</v>
-      </c>
-      <c r="H92" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I92" s="0" t="n">
-        <v>1</v>
       </c>
       <c r="R92" s="2"/>
     </row>

</xml_diff>